<commit_message>
Fixed the inputs of the excel sheets
</commit_message>
<xml_diff>
--- a/src/test/java/data/TestData.xlsx
+++ b/src/test/java/data/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4FFBFF15-72C3-40FB-92D2-63F0657F0C29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{83D3C3A0-8539-4D33-9269-52A048CCB28E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18690" windowHeight="6435" xr2:uid="{7801A892-92F3-4203-A84F-DF44FEE791BB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18420" windowHeight="6525" xr2:uid="{7801A892-92F3-4203-A84F-DF44FEE791BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>gender</t>
   </si>
@@ -53,13 +53,13 @@
     <t>male</t>
   </si>
   <si>
-    <t>Katheleen</t>
-  </si>
-  <si>
-    <t>Purdy</t>
-  </si>
-  <si>
-    <t>13</t>
+    <t>Brooks</t>
+  </si>
+  <si>
+    <t>Veum</t>
+  </si>
+  <si>
+    <t>24</t>
   </si>
   <si>
     <t>3</t>
@@ -68,31 +68,97 @@
     <t>2019</t>
   </si>
   <si>
-    <t>shawnda.schiller@yahoo.com</t>
-  </si>
-  <si>
-    <t>Heaney-Beier</t>
-  </si>
-  <si>
-    <t>rormj7x5</t>
-  </si>
-  <si>
-    <t>Tova</t>
-  </si>
-  <si>
-    <t>Olson</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>norman.hagenes@yahoo.com</t>
-  </si>
-  <si>
-    <t>Wunsch-Klocko</t>
-  </si>
-  <si>
-    <t>x4r60122</t>
+    <t>raleigh.collier@gmail.com</t>
+  </si>
+  <si>
+    <t>Beer-Larson</t>
+  </si>
+  <si>
+    <t>4v91czqfih6fa</t>
+  </si>
+  <si>
+    <t>Lyman</t>
+  </si>
+  <si>
+    <t>Beer</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>merilyn.keeling@hotmail.com</t>
+  </si>
+  <si>
+    <t>Heidenreich Group</t>
+  </si>
+  <si>
+    <t>0g7fduyw</t>
+  </si>
+  <si>
+    <t>Tad</t>
+  </si>
+  <si>
+    <t>Skiles</t>
+  </si>
+  <si>
+    <t>jayne.koepp@gmail.com</t>
+  </si>
+  <si>
+    <t>Christiansen, Thiel and Balistreri</t>
+  </si>
+  <si>
+    <t>ah51sitlk39e3ik</t>
+  </si>
+  <si>
+    <t>Timothy</t>
+  </si>
+  <si>
+    <t>Swift</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>andrew.daniel@yahoo.com</t>
+  </si>
+  <si>
+    <t>Lueilwitz, Lebsack and Krajcik</t>
+  </si>
+  <si>
+    <t>w6oe0es6d</t>
+  </si>
+  <si>
+    <t>Rosalva</t>
+  </si>
+  <si>
+    <t>Krajcik</t>
+  </si>
+  <si>
+    <t>molly.johnston@hotmail.com</t>
+  </si>
+  <si>
+    <t>Bradtke, Douglas and Mayer</t>
+  </si>
+  <si>
+    <t>joi1n6l1u5i14</t>
+  </si>
+  <si>
+    <t>Temeka</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>fairy.auer@hotmail.com</t>
+  </si>
+  <si>
+    <t>Kovacek-Doyle</t>
+  </si>
+  <si>
+    <t>6kpaqrwkzbc4k30</t>
   </si>
 </sst>
 </file>
@@ -445,19 +511,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656D4EE9-41F5-44C7-AC07-F0C875359FA8}">
-  <dimension ref="A2:I3"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,13 +564,13 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -506,13 +579,13 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -520,13 +593,13 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -535,15 +608,132 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed the excel issues
</commit_message>
<xml_diff>
--- a/src/test/java/data/TestData.xlsx
+++ b/src/test/java/data/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="213">
   <si>
     <t>gender</t>
   </si>
@@ -159,6 +159,507 @@
   </si>
   <si>
     <t>6kpaqrwkzbc4k30</t>
+  </si>
+  <si>
+    <t>Dorian</t>
+  </si>
+  <si>
+    <t>Parker</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>norris.jones@gmail.com</t>
+  </si>
+  <si>
+    <t>Goldner, Daniel and Bernier</t>
+  </si>
+  <si>
+    <t>xfwbcl0m</t>
+  </si>
+  <si>
+    <t>Rafaela</t>
+  </si>
+  <si>
+    <t>Feeney</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>cyrus.parisian@gmail.com</t>
+  </si>
+  <si>
+    <t>Mills LLC</t>
+  </si>
+  <si>
+    <t>hb0rwk4j</t>
+  </si>
+  <si>
+    <t>Bryon</t>
+  </si>
+  <si>
+    <t>Lindgren</t>
+  </si>
+  <si>
+    <t>jannette.okuneva@yahoo.com</t>
+  </si>
+  <si>
+    <t>Veum Inc</t>
+  </si>
+  <si>
+    <t>scvbl8os1bwg</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Muller</t>
+  </si>
+  <si>
+    <t>joey.flatley@hotmail.com</t>
+  </si>
+  <si>
+    <t>D'Amore, McDermott and Ziemann</t>
+  </si>
+  <si>
+    <t>c8shw30e9ck</t>
+  </si>
+  <si>
+    <t>Bunny</t>
+  </si>
+  <si>
+    <t>Shields</t>
+  </si>
+  <si>
+    <t>king.bernhard@hotmail.com</t>
+  </si>
+  <si>
+    <t>Ferry, Gusikowski and Hegmann</t>
+  </si>
+  <si>
+    <t>unadevmy9jeboz</t>
+  </si>
+  <si>
+    <t>Michelina</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>armando.lueilwitz@gmail.com</t>
+  </si>
+  <si>
+    <t>Ryan Group</t>
+  </si>
+  <si>
+    <t>3rtoxfwp2pq9ai8</t>
+  </si>
+  <si>
+    <t>Erma</t>
+  </si>
+  <si>
+    <t>Swaniawski</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>doug.wuckert@yahoo.com</t>
+  </si>
+  <si>
+    <t>Watsica and Sons</t>
+  </si>
+  <si>
+    <t>i95x97r8</t>
+  </si>
+  <si>
+    <t>Norbert</t>
+  </si>
+  <si>
+    <t>Kris</t>
+  </si>
+  <si>
+    <t>shaniqua.lockman@yahoo.com</t>
+  </si>
+  <si>
+    <t>Mertz-Schmidt</t>
+  </si>
+  <si>
+    <t>lnd02d578s</t>
+  </si>
+  <si>
+    <t>Loraine</t>
+  </si>
+  <si>
+    <t>Beatty</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>connie.larkin@hotmail.com</t>
+  </si>
+  <si>
+    <t>Bayer-Buckridge</t>
+  </si>
+  <si>
+    <t>8qp38ed4nxr2x</t>
+  </si>
+  <si>
+    <t>Ingeborg</t>
+  </si>
+  <si>
+    <t>Schoen</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>katelyn.krajcik@yahoo.com</t>
+  </si>
+  <si>
+    <t>Pfannerstill LLC</t>
+  </si>
+  <si>
+    <t>fco2fnzq</t>
+  </si>
+  <si>
+    <t>Maurice</t>
+  </si>
+  <si>
+    <t>Reichel</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>suzie.funk@yahoo.com</t>
+  </si>
+  <si>
+    <t>Wilderman-Reinger</t>
+  </si>
+  <si>
+    <t>su3abcv9l4cdzfv</t>
+  </si>
+  <si>
+    <t>Sherman</t>
+  </si>
+  <si>
+    <t>Moen</t>
+  </si>
+  <si>
+    <t>merlin.torphy@gmail.com</t>
+  </si>
+  <si>
+    <t>Ebert-Gottlieb</t>
+  </si>
+  <si>
+    <t>qn33bmy24pexq</t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>Osinski</t>
+  </si>
+  <si>
+    <t>micah.will@gmail.com</t>
+  </si>
+  <si>
+    <t>Hansen LLC</t>
+  </si>
+  <si>
+    <t>wlqr2zomev</t>
+  </si>
+  <si>
+    <t>Mack</t>
+  </si>
+  <si>
+    <t>Ondricka</t>
+  </si>
+  <si>
+    <t>arlene.doyle@yahoo.com</t>
+  </si>
+  <si>
+    <t>Von, Hartmann and Haley</t>
+  </si>
+  <si>
+    <t>33506jrghu</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>Rosenbaum</t>
+  </si>
+  <si>
+    <t>sharilyn.kuhn@hotmail.com</t>
+  </si>
+  <si>
+    <t>Dach, Friesen and Hoppe</t>
+  </si>
+  <si>
+    <t>068q2b5yf</t>
+  </si>
+  <si>
+    <t>Dianne</t>
+  </si>
+  <si>
+    <t>Hegmann</t>
+  </si>
+  <si>
+    <t>jerry.fisher@yahoo.com</t>
+  </si>
+  <si>
+    <t>Cormier and Sons</t>
+  </si>
+  <si>
+    <t>y6hi5ffvqm0z2tk</t>
+  </si>
+  <si>
+    <t>Cherelle</t>
+  </si>
+  <si>
+    <t>Harber</t>
+  </si>
+  <si>
+    <t>domenic.hane@gmail.com</t>
+  </si>
+  <si>
+    <t>Mitchell, Bernier and Wintheiser</t>
+  </si>
+  <si>
+    <t>s9sjc03ie4yt</t>
+  </si>
+  <si>
+    <t>Dionne</t>
+  </si>
+  <si>
+    <t>Nitzsche</t>
+  </si>
+  <si>
+    <t>chad.muller@yahoo.com</t>
+  </si>
+  <si>
+    <t>Oberbrunner Inc</t>
+  </si>
+  <si>
+    <t>fu7dzs3a693y</t>
+  </si>
+  <si>
+    <t>Harley</t>
+  </si>
+  <si>
+    <t>Crooks</t>
+  </si>
+  <si>
+    <t>clint.vandervort@yahoo.com</t>
+  </si>
+  <si>
+    <t>Herzog, Jast and Christiansen</t>
+  </si>
+  <si>
+    <t>yij08y5b0</t>
+  </si>
+  <si>
+    <t>Trevor</t>
+  </si>
+  <si>
+    <t>Marvin</t>
+  </si>
+  <si>
+    <t>tracy.stamm@yahoo.com</t>
+  </si>
+  <si>
+    <t>Rohan Inc</t>
+  </si>
+  <si>
+    <t>14rz8z6q70na</t>
+  </si>
+  <si>
+    <t>Mathew</t>
+  </si>
+  <si>
+    <t>Lehner</t>
+  </si>
+  <si>
+    <t>paul.harvey@hotmail.com</t>
+  </si>
+  <si>
+    <t>Stanton Inc</t>
+  </si>
+  <si>
+    <t>87zj4we328mez</t>
+  </si>
+  <si>
+    <t>Margorie</t>
+  </si>
+  <si>
+    <t>domingo.wyman@yahoo.com</t>
+  </si>
+  <si>
+    <t>Fahey, Paucek and Kuhn</t>
+  </si>
+  <si>
+    <t>u3i2y49w5k4czqc</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Gorczany</t>
+  </si>
+  <si>
+    <t>adalberto.spinka@hotmail.com</t>
+  </si>
+  <si>
+    <t>Terry, Parker and Rowe</t>
+  </si>
+  <si>
+    <t>mcoy7zvodlpbgn4</t>
+  </si>
+  <si>
+    <t>Tomas</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>nick.luettgen@hotmail.com</t>
+  </si>
+  <si>
+    <t>Bashirian-Becker</t>
+  </si>
+  <si>
+    <t>2exj6nd1qq4du4</t>
+  </si>
+  <si>
+    <t>Chloe</t>
+  </si>
+  <si>
+    <t>Larson</t>
+  </si>
+  <si>
+    <t>emilie.frami@hotmail.com</t>
+  </si>
+  <si>
+    <t>Jacobi-Hettinger</t>
+  </si>
+  <si>
+    <t>72qoymoxib372u</t>
+  </si>
+  <si>
+    <t>Jaclyn</t>
+  </si>
+  <si>
+    <t>Hirthe</t>
+  </si>
+  <si>
+    <t>lanie.will@hotmail.com</t>
+  </si>
+  <si>
+    <t>Hauck, Haley and Lang</t>
+  </si>
+  <si>
+    <t>b23kod7in4fo3</t>
+  </si>
+  <si>
+    <t>Vernon</t>
+  </si>
+  <si>
+    <t>Rolfson</t>
+  </si>
+  <si>
+    <t>yasmine.goodwin@hotmail.com</t>
+  </si>
+  <si>
+    <t>Mayert, Cassin and Turcotte</t>
+  </si>
+  <si>
+    <t>jq7bupm8ikj6</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>katelynn.bergnaum@gmail.com</t>
+  </si>
+  <si>
+    <t>Becker LLC</t>
+  </si>
+  <si>
+    <t>0e0b9lreyms3</t>
+  </si>
+  <si>
+    <t>Cortez</t>
+  </si>
+  <si>
+    <t>Olson</t>
+  </si>
+  <si>
+    <t>casey.thompson@hotmail.com</t>
+  </si>
+  <si>
+    <t>Moore Group</t>
+  </si>
+  <si>
+    <t>7h62yjamdjf</t>
+  </si>
+  <si>
+    <t>Cecil</t>
+  </si>
+  <si>
+    <t>O'Kon</t>
+  </si>
+  <si>
+    <t>shawnna.strosin@gmail.com</t>
+  </si>
+  <si>
+    <t>Ruecker Group</t>
+  </si>
+  <si>
+    <t>ue592kiios88uf</t>
+  </si>
+  <si>
+    <t>Stacy</t>
+  </si>
+  <si>
+    <t>Cassin</t>
+  </si>
+  <si>
+    <t>dion.bogisich@gmail.com</t>
+  </si>
+  <si>
+    <t>Thiel, Heathcote and Jerde</t>
+  </si>
+  <si>
+    <t>im77t5d7rkimrf</t>
+  </si>
+  <si>
+    <t>Lacy</t>
+  </si>
+  <si>
+    <t>newton.yost@hotmail.com</t>
+  </si>
+  <si>
+    <t>Collins, Swaniawski and Dach</t>
+  </si>
+  <si>
+    <t>bxy90qp7q3f7</t>
   </si>
 </sst>
 </file>
@@ -564,10 +1065,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>184</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>185</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -579,13 +1080,13 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>186</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>187</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3">
@@ -593,13 +1094,13 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>170</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -608,13 +1109,13 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>191</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>192</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4">
@@ -622,13 +1123,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>194</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>195</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -637,13 +1138,13 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>196</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>197</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5">
@@ -651,13 +1152,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -666,13 +1167,13 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>201</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>202</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6">
@@ -680,13 +1181,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>204</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>205</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -695,13 +1196,13 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>206</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>207</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7">
@@ -709,13 +1210,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>209</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -724,13 +1225,13 @@
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>210</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>211</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working on reading the user name and password from excel sheet
</commit_message>
<xml_diff>
--- a/src/test/java/data/TestData.xlsx
+++ b/src/test/java/data/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="930">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="958">
   <si>
     <t>gender</t>
   </si>
@@ -2811,6 +2811,90 @@
   </si>
   <si>
     <t>nzzck85wzqgi</t>
+  </si>
+  <si>
+    <t>Koelpin</t>
+  </si>
+  <si>
+    <t>gordon.grady@hotmail.com</t>
+  </si>
+  <si>
+    <t>Gottlieb Inc</t>
+  </si>
+  <si>
+    <t>zzklx9z4e</t>
+  </si>
+  <si>
+    <t>Miranda</t>
+  </si>
+  <si>
+    <t>Steuber</t>
+  </si>
+  <si>
+    <t>luther.goldner@gmail.com</t>
+  </si>
+  <si>
+    <t>Shields, Adams and Kemmer</t>
+  </si>
+  <si>
+    <t>zfjcn4g24jpf</t>
+  </si>
+  <si>
+    <t>Margarito</t>
+  </si>
+  <si>
+    <t>Corwin</t>
+  </si>
+  <si>
+    <t>cecil.smitham@yahoo.com</t>
+  </si>
+  <si>
+    <t>Ullrich, Bins and Sauer</t>
+  </si>
+  <si>
+    <t>4jzty0p6u</t>
+  </si>
+  <si>
+    <t>Antony</t>
+  </si>
+  <si>
+    <t>Schmeler</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>fred.sanford@gmail.com</t>
+  </si>
+  <si>
+    <t>Kihn, Gibson and Cremin</t>
+  </si>
+  <si>
+    <t>8bgpvktgwzop</t>
+  </si>
+  <si>
+    <t>Nicholas</t>
+  </si>
+  <si>
+    <t>lazaro.carter@yahoo.com</t>
+  </si>
+  <si>
+    <t>Cronin, King and Windler</t>
+  </si>
+  <si>
+    <t>ruf0s21109ffa</t>
+  </si>
+  <si>
+    <t>Dolly</t>
+  </si>
+  <si>
+    <t>cyril.lueilwitz@gmail.com</t>
+  </si>
+  <si>
+    <t>Rempel and Sons</t>
+  </si>
+  <si>
+    <t>dwdtwivdq2xnn</t>
   </si>
 </sst>
 </file>
@@ -3216,13 +3300,13 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>900</v>
+        <v>844</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>930</v>
       </c>
       <c r="D2" t="s">
-        <v>901</v>
+        <v>170</v>
       </c>
       <c r="E2" t="s">
         <v>105</v>
@@ -3231,13 +3315,13 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>902</v>
+        <v>931</v>
       </c>
       <c r="H2" t="s">
-        <v>903</v>
+        <v>932</v>
       </c>
       <c r="I2" t="s">
-        <v>904</v>
+        <v>933</v>
       </c>
     </row>
     <row r="3">
@@ -3245,28 +3329,28 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>905</v>
+        <v>934</v>
       </c>
       <c r="C3" t="s">
-        <v>906</v>
+        <v>935</v>
       </c>
       <c r="D3" t="s">
         <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>907</v>
+        <v>936</v>
       </c>
       <c r="H3" t="s">
-        <v>908</v>
+        <v>937</v>
       </c>
       <c r="I3" t="s">
-        <v>909</v>
+        <v>938</v>
       </c>
     </row>
     <row r="4">
@@ -3274,13 +3358,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>910</v>
+        <v>939</v>
       </c>
       <c r="C4" t="s">
-        <v>911</v>
+        <v>940</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
         <v>105</v>
@@ -3289,13 +3373,13 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>912</v>
+        <v>941</v>
       </c>
       <c r="H4" t="s">
-        <v>913</v>
+        <v>942</v>
       </c>
       <c r="I4" t="s">
-        <v>914</v>
+        <v>943</v>
       </c>
     </row>
     <row r="5">
@@ -3303,28 +3387,28 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>915</v>
+        <v>944</v>
       </c>
       <c r="C5" t="s">
-        <v>916</v>
+        <v>945</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>946</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>220</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>917</v>
+        <v>947</v>
       </c>
       <c r="H5" t="s">
-        <v>918</v>
+        <v>948</v>
       </c>
       <c r="I5" t="s">
-        <v>919</v>
+        <v>949</v>
       </c>
     </row>
     <row r="6">
@@ -3332,28 +3416,28 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>920</v>
+        <v>950</v>
       </c>
       <c r="C6" t="s">
-        <v>921</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>922</v>
+        <v>951</v>
       </c>
       <c r="H6" t="s">
-        <v>923</v>
+        <v>952</v>
       </c>
       <c r="I6" t="s">
-        <v>924</v>
+        <v>953</v>
       </c>
     </row>
     <row r="7">
@@ -3361,28 +3445,28 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>925</v>
+        <v>954</v>
       </c>
       <c r="C7" t="s">
-        <v>926</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>220</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>927</v>
+        <v>955</v>
       </c>
       <c r="H7" t="s">
-        <v>928</v>
+        <v>956</v>
       </c>
       <c r="I7" t="s">
-        <v>929</v>
+        <v>957</v>
       </c>
     </row>
     <row r="8" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>